<commit_message>
schema d'architecture et tâches
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Tâches</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Créer le programme qui va collectecter les données et les inscrires dans les fichiers texte</t>
+  </si>
+  <si>
+    <t>Les deux</t>
+  </si>
+  <si>
+    <t>En attente</t>
   </si>
 </sst>
 </file>
@@ -199,12 +205,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,20 +498,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="C3:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -529,171 +535,198 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="str">
+      <c r="F4" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="4" t="str">
         <f>Etat!C2</f>
         <v>Fait</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="str">
+      <c r="F5" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5" t="str">
+      <c r="F6" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="str">
+      <c r="F7" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5" t="str">
+      <c r="F8" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5" t="str">
+      <c r="F9" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="5">
+      <c r="F10" s="4" t="str">
+        <f>Participants!A3</f>
+        <v>Alexandre Bodart</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="5">
+      <c r="F11" s="4" t="str">
+        <f>Participants!A3</f>
+        <v>Alexandre Bodart</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="5" t="str">
+      <c r="F12" s="4" t="str">
         <f>Participants!A2</f>
         <v>François Monteil</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H12" s="4">
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f>Participants!A2</f>
+        <v>François Monteil</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="14" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="5">
+      <c r="F14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="4">
         <v>10</v>
       </c>
     </row>
@@ -767,17 +800,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>